<commit_message>
improved ui, added locate me button, light and surface filter, icons, clean search, nav via google and waze, details on each court
</commit_message>
<xml_diff>
--- a/backend/COURTS.xlsx
+++ b/backend/COURTS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinzu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinzu\migrash\migrash\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594ADA0B-8AFA-48E9-A61E-573F8B63C9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDBD791-F87D-4AB5-B3CE-24250F0ADDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,6 +54,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>תומר ארצי:
@@ -68,6 +69,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>תומר ארצי:
@@ -82,6 +84,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>תומר ארצי:
@@ -96,6 +99,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>תומר ארצי:
@@ -110,6 +114,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>תומר ארצי:
@@ -134,6 +139,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>תומר ארצי:
@@ -148,6 +154,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>תומר ארצי:
@@ -162,6 +169,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>תומר ארצי:
@@ -176,6 +184,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>תומר ארצי:
@@ -190,6 +199,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>תומר ארצי:
@@ -202,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5646" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5646" uniqueCount="842">
   <si>
     <t xml:space="preserve">נתוני מיתקן </t>
   </si>
@@ -2976,6 +2986,18 @@
   </si>
   <si>
     <t>מתקן פתוח לכושר גופני</t>
+  </si>
+  <si>
+    <t>Basketball court</t>
+  </si>
+  <si>
+    <t>Football court</t>
+  </si>
+  <si>
+    <t>Multi-purpose court</t>
+  </si>
+  <si>
+    <t>Volleyball court</t>
   </si>
 </sst>
 </file>
@@ -11889,7 +11911,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11956,7 +11978,7 @@
         <v>18</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>309</v>
@@ -11994,7 +12016,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>309</v>
@@ -12032,7 +12054,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>309</v>
@@ -12070,7 +12092,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>309</v>
@@ -12108,7 +12130,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>309</v>
@@ -12146,7 +12168,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>309</v>
@@ -12184,7 +12206,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>309</v>
@@ -12222,7 +12244,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>309</v>
@@ -12260,7 +12282,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>309</v>
@@ -12298,7 +12320,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>309</v>
@@ -12336,7 +12358,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>309</v>
@@ -12374,7 +12396,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>309</v>
@@ -12412,7 +12434,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>309</v>
@@ -12450,7 +12472,7 @@
         <v>18</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>309</v>
@@ -12488,7 +12510,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>309</v>
@@ -12526,7 +12548,7 @@
         <v>18</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>309</v>
@@ -12564,7 +12586,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>309</v>
@@ -12602,7 +12624,7 @@
         <v>18</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>309</v>
@@ -12640,7 +12662,7 @@
         <v>18</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>309</v>
@@ -12678,7 +12700,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>309</v>
@@ -12716,7 +12738,7 @@
         <v>18</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>309</v>
@@ -12754,7 +12776,7 @@
         <v>18</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>309</v>
@@ -12792,7 +12814,7 @@
         <v>18</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>309</v>
@@ -12830,7 +12852,7 @@
         <v>18</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>309</v>
@@ -12868,7 +12890,7 @@
         <v>18</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>309</v>
@@ -12906,7 +12928,7 @@
         <v>18</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>309</v>
@@ -12944,7 +12966,7 @@
         <v>18</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>309</v>
@@ -12982,7 +13004,7 @@
         <v>18</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>309</v>
@@ -13020,7 +13042,7 @@
         <v>18</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>309</v>
@@ -13058,7 +13080,7 @@
         <v>18</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>309</v>
@@ -13096,7 +13118,7 @@
         <v>18</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>309</v>
@@ -13134,7 +13156,7 @@
         <v>18</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>309</v>
@@ -13172,7 +13194,7 @@
         <v>18</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>309</v>
@@ -13210,7 +13232,7 @@
         <v>18</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>309</v>
@@ -13248,7 +13270,7 @@
         <v>18</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>309</v>
@@ -13286,7 +13308,7 @@
         <v>18</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>309</v>
@@ -13324,7 +13346,7 @@
         <v>18</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>309</v>
@@ -13362,7 +13384,7 @@
         <v>18</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>309</v>
@@ -13400,7 +13422,7 @@
         <v>18</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>309</v>
@@ -13438,7 +13460,7 @@
         <v>18</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>309</v>
@@ -13476,7 +13498,7 @@
         <v>18</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>309</v>
@@ -13514,7 +13536,7 @@
         <v>18</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>309</v>
@@ -13552,7 +13574,7 @@
         <v>18</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>309</v>
@@ -13590,7 +13612,7 @@
         <v>18</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>309</v>
@@ -13628,7 +13650,7 @@
         <v>18</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>309</v>
@@ -13666,7 +13688,7 @@
         <v>18</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>309</v>
@@ -13704,7 +13726,7 @@
         <v>18</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>309</v>
@@ -13742,7 +13764,7 @@
         <v>18</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>309</v>
@@ -13780,7 +13802,7 @@
         <v>18</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>309</v>
@@ -13818,7 +13840,7 @@
         <v>18</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>309</v>
@@ -13854,7 +13876,7 @@
         <v>18</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>309</v>
@@ -13890,7 +13912,7 @@
         <v>18</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>309</v>
@@ -13926,7 +13948,7 @@
         <v>18</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>309</v>
@@ -13964,7 +13986,7 @@
         <v>18</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>309</v>
@@ -14002,7 +14024,7 @@
         <v>18</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>309</v>
@@ -14040,7 +14062,7 @@
         <v>18</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>309</v>
@@ -14078,7 +14100,7 @@
         <v>18</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>309</v>
@@ -14116,7 +14138,7 @@
         <v>18</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>309</v>
@@ -14154,7 +14176,7 @@
         <v>18</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>309</v>
@@ -14192,7 +14214,7 @@
         <v>18</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>309</v>
@@ -14226,7 +14248,7 @@
         <v>18</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>309</v>
@@ -14260,7 +14282,7 @@
         <v>18</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>309</v>
@@ -14298,7 +14320,7 @@
         <v>18</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>309</v>
@@ -14336,7 +14358,7 @@
         <v>18</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>309</v>
@@ -14374,7 +14396,7 @@
         <v>18</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>309</v>
@@ -14412,7 +14434,7 @@
         <v>18</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>309</v>
@@ -14450,7 +14472,7 @@
         <v>18</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>309</v>
@@ -14488,7 +14510,7 @@
         <v>18</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>309</v>
@@ -14526,7 +14548,7 @@
         <v>18</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>309</v>
@@ -14564,7 +14586,7 @@
         <v>18</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>309</v>
@@ -14602,7 +14624,7 @@
         <v>18</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>309</v>
@@ -14640,7 +14662,7 @@
         <v>18</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>309</v>
@@ -14678,7 +14700,7 @@
         <v>18</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>309</v>
@@ -14716,7 +14738,7 @@
         <v>18</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>309</v>
@@ -14754,7 +14776,7 @@
         <v>18</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>309</v>
@@ -14792,7 +14814,7 @@
         <v>18</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>309</v>
@@ -14830,7 +14852,7 @@
         <v>18</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>309</v>
@@ -14868,7 +14890,7 @@
         <v>18</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>309</v>
@@ -14906,7 +14928,7 @@
         <v>18</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>309</v>
@@ -14944,7 +14966,7 @@
         <v>18</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>309</v>
@@ -14982,7 +15004,7 @@
         <v>18</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>309</v>
@@ -15020,7 +15042,7 @@
         <v>18</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>309</v>
@@ -15058,7 +15080,7 @@
         <v>18</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>309</v>
@@ -15096,7 +15118,7 @@
         <v>18</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>309</v>
@@ -15134,7 +15156,7 @@
         <v>18</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>309</v>
@@ -15172,7 +15194,7 @@
         <v>18</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>309</v>
@@ -15210,7 +15232,7 @@
         <v>18</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>309</v>
@@ -15246,7 +15268,7 @@
         <v>18</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>309</v>
@@ -15282,7 +15304,7 @@
         <v>18</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>309</v>
@@ -15318,7 +15340,7 @@
         <v>18</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>309</v>
@@ -15354,7 +15376,7 @@
         <v>18</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>309</v>
@@ -15390,7 +15412,7 @@
         <v>18</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>309</v>
@@ -15426,7 +15448,7 @@
         <v>18</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>309</v>
@@ -15462,7 +15484,7 @@
         <v>18</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>309</v>
@@ -15498,7 +15520,7 @@
         <v>18</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>309</v>
@@ -15534,7 +15556,7 @@
         <v>18</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>309</v>
@@ -15570,7 +15592,7 @@
         <v>18</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>309</v>
@@ -15604,7 +15626,7 @@
         <v>18</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>309</v>
@@ -15638,7 +15660,7 @@
         <v>18</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>309</v>
@@ -15672,7 +15694,7 @@
         <v>18</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>309</v>
@@ -15706,7 +15728,7 @@
         <v>18</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>314</v>
@@ -15740,7 +15762,7 @@
         <v>18</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>309</v>
@@ -15774,7 +15796,7 @@
         <v>18</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E104" s="8" t="s">
         <v>309</v>
@@ -15810,7 +15832,7 @@
         <v>18</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>309</v>
@@ -15846,7 +15868,7 @@
         <v>18</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>309</v>
@@ -15882,7 +15904,7 @@
         <v>18</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>309</v>
@@ -15918,7 +15940,7 @@
         <v>18</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E108" s="8" t="s">
         <v>309</v>
@@ -15954,7 +15976,7 @@
         <v>18</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>309</v>
@@ -15990,7 +16012,7 @@
         <v>18</v>
       </c>
       <c r="D110" s="14" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>309</v>
@@ -16026,7 +16048,7 @@
         <v>18</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>309</v>
@@ -16060,7 +16082,7 @@
         <v>18</v>
       </c>
       <c r="D112" s="14" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E112" s="8" t="s">
         <v>309</v>
@@ -16094,7 +16116,7 @@
         <v>18</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>309</v>
@@ -16128,7 +16150,7 @@
         <v>18</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>309</v>
@@ -16164,7 +16186,7 @@
         <v>18</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>309</v>
@@ -16200,7 +16222,7 @@
         <v>18</v>
       </c>
       <c r="D116" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>309</v>
@@ -16236,7 +16258,7 @@
         <v>18</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>309</v>
@@ -16272,7 +16294,7 @@
         <v>18</v>
       </c>
       <c r="D118" s="14" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>309</v>
@@ -16308,7 +16330,7 @@
         <v>18</v>
       </c>
       <c r="D119" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E119" s="8" t="s">
         <v>309</v>
@@ -16344,7 +16366,7 @@
         <v>18</v>
       </c>
       <c r="D120" s="14" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>309</v>
@@ -16380,7 +16402,7 @@
         <v>18</v>
       </c>
       <c r="D121" s="14" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>309</v>
@@ -16416,7 +16438,7 @@
         <v>18</v>
       </c>
       <c r="D122" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>309</v>
@@ -16452,7 +16474,7 @@
         <v>18</v>
       </c>
       <c r="D123" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>309</v>
@@ -16486,7 +16508,7 @@
         <v>18</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>309</v>
@@ -16520,7 +16542,7 @@
         <v>18</v>
       </c>
       <c r="D125" s="14" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E125" s="8" t="s">
         <v>309</v>
@@ -16554,7 +16576,7 @@
         <v>18</v>
       </c>
       <c r="D126" s="14" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E126" s="8" t="s">
         <v>309</v>
@@ -16588,7 +16610,7 @@
         <v>18</v>
       </c>
       <c r="D127" s="14" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>309</v>
@@ -16622,7 +16644,7 @@
         <v>18</v>
       </c>
       <c r="D128" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E128" s="8" t="s">
         <v>309</v>
@@ -16652,7 +16674,7 @@
         <v>18</v>
       </c>
       <c r="D129" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>309</v>
@@ -16686,7 +16708,7 @@
         <v>18</v>
       </c>
       <c r="D130" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E130" s="8" t="s">
         <v>309</v>
@@ -16720,7 +16742,7 @@
         <v>18</v>
       </c>
       <c r="D131" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>309</v>
@@ -16754,7 +16776,7 @@
         <v>18</v>
       </c>
       <c r="D132" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E132" s="8" t="s">
         <v>309</v>
@@ -16788,7 +16810,7 @@
         <v>18</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E133" s="8" t="s">
         <v>309</v>
@@ -16822,7 +16844,7 @@
         <v>18</v>
       </c>
       <c r="D134" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E134" s="8" t="s">
         <v>309</v>
@@ -16856,7 +16878,7 @@
         <v>18</v>
       </c>
       <c r="D135" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E135" s="8" t="s">
         <v>309</v>
@@ -16886,7 +16908,7 @@
         <v>18</v>
       </c>
       <c r="D136" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E136" s="8" t="s">
         <v>309</v>
@@ -16920,7 +16942,7 @@
         <v>18</v>
       </c>
       <c r="D137" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E137" s="8" t="s">
         <v>309</v>
@@ -16954,7 +16976,7 @@
         <v>18</v>
       </c>
       <c r="D138" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E138" s="8" t="s">
         <v>309</v>
@@ -16988,7 +17010,7 @@
         <v>18</v>
       </c>
       <c r="D139" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E139" s="8" t="s">
         <v>309</v>
@@ -17022,7 +17044,7 @@
         <v>18</v>
       </c>
       <c r="D140" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E140" s="8" t="s">
         <v>309</v>
@@ -17056,7 +17078,7 @@
         <v>18</v>
       </c>
       <c r="D141" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E141" s="8" t="s">
         <v>309</v>
@@ -17090,7 +17112,7 @@
         <v>18</v>
       </c>
       <c r="D142" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E142" s="8" t="s">
         <v>309</v>
@@ -17124,7 +17146,7 @@
         <v>18</v>
       </c>
       <c r="D143" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E143" s="8" t="s">
         <v>309</v>
@@ -17158,7 +17180,7 @@
         <v>18</v>
       </c>
       <c r="D144" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E144" s="8" t="s">
         <v>309</v>
@@ -17192,7 +17214,7 @@
         <v>18</v>
       </c>
       <c r="D145" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E145" s="8" t="s">
         <v>309</v>
@@ -17226,7 +17248,7 @@
         <v>18</v>
       </c>
       <c r="D146" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E146" s="8" t="s">
         <v>309</v>
@@ -17260,7 +17282,7 @@
         <v>18</v>
       </c>
       <c r="D147" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E147" s="8" t="s">
         <v>309</v>
@@ -17294,7 +17316,7 @@
         <v>18</v>
       </c>
       <c r="D148" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E148" s="8" t="s">
         <v>309</v>
@@ -17328,7 +17350,7 @@
         <v>18</v>
       </c>
       <c r="D149" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E149" s="8" t="s">
         <v>309</v>
@@ -17362,7 +17384,7 @@
         <v>18</v>
       </c>
       <c r="D150" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E150" s="8" t="s">
         <v>309</v>
@@ -17396,7 +17418,7 @@
         <v>18</v>
       </c>
       <c r="D151" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E151" s="8" t="s">
         <v>309</v>
@@ -17430,7 +17452,7 @@
         <v>18</v>
       </c>
       <c r="D152" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E152" s="8" t="s">
         <v>309</v>
@@ -17460,7 +17482,7 @@
         <v>18</v>
       </c>
       <c r="D153" s="29" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E153" s="8" t="s">
         <v>309</v>
@@ -17494,7 +17516,7 @@
         <v>18</v>
       </c>
       <c r="D154" s="8" t="s">
-        <v>308</v>
+        <v>838</v>
       </c>
       <c r="E154" s="8" t="s">
         <v>309</v>
@@ -17526,7 +17548,7 @@
         <v>18</v>
       </c>
       <c r="D155" s="8" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E155" s="8" t="s">
         <v>309</v>
@@ -17558,7 +17580,7 @@
         <v>18</v>
       </c>
       <c r="D156" s="29" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E156" s="8" t="s">
         <v>309</v>
@@ -17592,7 +17614,7 @@
         <v>18</v>
       </c>
       <c r="D157" s="29" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E157" s="8" t="s">
         <v>309</v>
@@ -17626,7 +17648,7 @@
         <v>18</v>
       </c>
       <c r="D158" s="29" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E158" s="8" t="s">
         <v>309</v>
@@ -17660,7 +17682,7 @@
         <v>18</v>
       </c>
       <c r="D159" s="29" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E159" s="8" t="s">
         <v>309</v>
@@ -17694,7 +17716,7 @@
         <v>18</v>
       </c>
       <c r="D160" s="29" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E160" s="8" t="s">
         <v>309</v>
@@ -17728,7 +17750,7 @@
         <v>18</v>
       </c>
       <c r="D161" s="29" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E161" s="8" t="s">
         <v>309</v>
@@ -17758,7 +17780,7 @@
         <v>18</v>
       </c>
       <c r="D162" s="29" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E162" s="8" t="s">
         <v>309</v>
@@ -17788,7 +17810,7 @@
         <v>18</v>
       </c>
       <c r="D163" s="29" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E163" s="8" t="s">
         <v>309</v>
@@ -17818,7 +17840,7 @@
         <v>18</v>
       </c>
       <c r="D164" s="29" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E164" s="8" t="s">
         <v>309</v>
@@ -17848,7 +17870,7 @@
         <v>18</v>
       </c>
       <c r="D165" s="29" t="s">
-        <v>312</v>
+        <v>840</v>
       </c>
       <c r="E165" s="8" t="s">
         <v>309</v>
@@ -17878,7 +17900,7 @@
         <v>18</v>
       </c>
       <c r="D166" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E166" s="8" t="s">
         <v>309</v>
@@ -17908,7 +17930,7 @@
         <v>18</v>
       </c>
       <c r="D167" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E167" s="8" t="s">
         <v>309</v>
@@ -17938,7 +17960,7 @@
         <v>18</v>
       </c>
       <c r="D168" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E168" s="8" t="s">
         <v>309</v>
@@ -17968,7 +17990,7 @@
         <v>18</v>
       </c>
       <c r="D169" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E169" s="8" t="s">
         <v>309</v>
@@ -17998,7 +18020,7 @@
         <v>18</v>
       </c>
       <c r="D170" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E170" s="8" t="s">
         <v>309</v>
@@ -18028,7 +18050,7 @@
         <v>18</v>
       </c>
       <c r="D171" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E171" s="8" t="s">
         <v>309</v>
@@ -18058,7 +18080,7 @@
         <v>18</v>
       </c>
       <c r="D172" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E172" s="8" t="s">
         <v>309</v>
@@ -18088,7 +18110,7 @@
         <v>18</v>
       </c>
       <c r="D173" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E173" s="8" t="s">
         <v>309</v>
@@ -18118,7 +18140,7 @@
         <v>18</v>
       </c>
       <c r="D174" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E174" s="8" t="s">
         <v>309</v>
@@ -18148,7 +18170,7 @@
         <v>18</v>
       </c>
       <c r="D175" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E175" s="8" t="s">
         <v>309</v>
@@ -18178,7 +18200,7 @@
         <v>18</v>
       </c>
       <c r="D176" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E176" s="8" t="s">
         <v>309</v>
@@ -18208,7 +18230,7 @@
         <v>18</v>
       </c>
       <c r="D177" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E177" s="8" t="s">
         <v>309</v>
@@ -18238,7 +18260,7 @@
         <v>18</v>
       </c>
       <c r="D178" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E178" s="8" t="s">
         <v>365</v>
@@ -18268,7 +18290,7 @@
         <v>18</v>
       </c>
       <c r="D179" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E179" s="8" t="s">
         <v>365</v>
@@ -18298,7 +18320,7 @@
         <v>18</v>
       </c>
       <c r="D180" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E180" s="8" t="s">
         <v>309</v>
@@ -18328,7 +18350,7 @@
         <v>18</v>
       </c>
       <c r="D181" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E181" s="8" t="s">
         <v>365</v>
@@ -18358,7 +18380,7 @@
         <v>18</v>
       </c>
       <c r="D182" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E182" s="8" t="s">
         <v>314</v>
@@ -18390,7 +18412,7 @@
         <v>18</v>
       </c>
       <c r="D183" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E183" s="8" t="s">
         <v>314</v>
@@ -18422,7 +18444,7 @@
         <v>18</v>
       </c>
       <c r="D184" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E184" s="8" t="s">
         <v>314</v>
@@ -18454,7 +18476,7 @@
         <v>18</v>
       </c>
       <c r="D185" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E185" s="8" t="s">
         <v>314</v>
@@ -18486,7 +18508,7 @@
         <v>18</v>
       </c>
       <c r="D186" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E186" s="8" t="s">
         <v>314</v>
@@ -18518,7 +18540,7 @@
         <v>18</v>
       </c>
       <c r="D187" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E187" s="8" t="s">
         <v>314</v>
@@ -18550,7 +18572,7 @@
         <v>18</v>
       </c>
       <c r="D188" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E188" s="8" t="s">
         <v>314</v>
@@ -18582,7 +18604,7 @@
         <v>18</v>
       </c>
       <c r="D189" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E189" s="8" t="s">
         <v>314</v>
@@ -18614,7 +18636,7 @@
         <v>18</v>
       </c>
       <c r="D190" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E190" s="8" t="s">
         <v>314</v>
@@ -18648,7 +18670,7 @@
         <v>18</v>
       </c>
       <c r="D191" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E191" s="8" t="s">
         <v>314</v>
@@ -18680,7 +18702,7 @@
         <v>18</v>
       </c>
       <c r="D192" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E192" s="8" t="s">
         <v>314</v>
@@ -18712,7 +18734,7 @@
         <v>18</v>
       </c>
       <c r="D193" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E193" s="8" t="s">
         <v>314</v>
@@ -18744,7 +18766,7 @@
         <v>18</v>
       </c>
       <c r="D194" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>314</v>
@@ -18776,7 +18798,7 @@
         <v>18</v>
       </c>
       <c r="D195" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E195" s="8" t="s">
         <v>314</v>
@@ -18808,7 +18830,7 @@
         <v>18</v>
       </c>
       <c r="D196" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E196" s="8" t="s">
         <v>314</v>
@@ -18840,7 +18862,7 @@
         <v>18</v>
       </c>
       <c r="D197" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>314</v>
@@ -18874,7 +18896,7 @@
         <v>18</v>
       </c>
       <c r="D198" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E198" s="8" t="s">
         <v>314</v>
@@ -18908,7 +18930,7 @@
         <v>18</v>
       </c>
       <c r="D199" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>314</v>
@@ -18942,7 +18964,7 @@
         <v>18</v>
       </c>
       <c r="D200" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>314</v>
@@ -18976,7 +18998,7 @@
         <v>18</v>
       </c>
       <c r="D201" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E201" s="8" t="s">
         <v>314</v>
@@ -19010,7 +19032,7 @@
         <v>18</v>
       </c>
       <c r="D202" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E202" s="8" t="s">
         <v>314</v>
@@ -19044,7 +19066,7 @@
         <v>18</v>
       </c>
       <c r="D203" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E203" s="8" t="s">
         <v>314</v>
@@ -19078,7 +19100,7 @@
         <v>18</v>
       </c>
       <c r="D204" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E204" s="8" t="s">
         <v>314</v>
@@ -19112,7 +19134,7 @@
         <v>18</v>
       </c>
       <c r="D205" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E205" s="8" t="s">
         <v>314</v>
@@ -19146,7 +19168,7 @@
         <v>18</v>
       </c>
       <c r="D206" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E206" s="8" t="s">
         <v>314</v>
@@ -19180,7 +19202,7 @@
         <v>18</v>
       </c>
       <c r="D207" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E207" s="8" t="s">
         <v>314</v>
@@ -19214,7 +19236,7 @@
         <v>18</v>
       </c>
       <c r="D208" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E208" s="8" t="s">
         <v>314</v>
@@ -19248,7 +19270,7 @@
         <v>18</v>
       </c>
       <c r="D209" s="29" t="s">
-        <v>313</v>
+        <v>841</v>
       </c>
       <c r="E209" s="8" t="s">
         <v>314</v>
@@ -19282,7 +19304,7 @@
         <v>381</v>
       </c>
       <c r="D210" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E210" s="8" t="s">
         <v>365</v>
@@ -19311,7 +19333,7 @@
         <v>381</v>
       </c>
       <c r="D211" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E211" s="8" t="s">
         <v>365</v>
@@ -19340,7 +19362,7 @@
         <v>381</v>
       </c>
       <c r="D212" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E212" s="8" t="s">
         <v>365</v>
@@ -19369,7 +19391,7 @@
         <v>381</v>
       </c>
       <c r="D213" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E213" s="8" t="s">
         <v>365</v>
@@ -19398,7 +19420,7 @@
         <v>381</v>
       </c>
       <c r="D214" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E214" s="8" t="s">
         <v>365</v>
@@ -19427,7 +19449,7 @@
         <v>381</v>
       </c>
       <c r="D215" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E215" s="8" t="s">
         <v>365</v>
@@ -19456,7 +19478,7 @@
         <v>381</v>
       </c>
       <c r="D216" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E216" s="8" t="s">
         <v>365</v>
@@ -19485,7 +19507,7 @@
         <v>381</v>
       </c>
       <c r="D217" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E217" s="8" t="s">
         <v>365</v>
@@ -19514,7 +19536,7 @@
         <v>381</v>
       </c>
       <c r="D218" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E218" s="8" t="s">
         <v>365</v>
@@ -19543,7 +19565,7 @@
         <v>381</v>
       </c>
       <c r="D219" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E219" s="8" t="s">
         <v>365</v>
@@ -19572,7 +19594,7 @@
         <v>384</v>
       </c>
       <c r="D220" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E220" s="8" t="s">
         <v>365</v>
@@ -19601,7 +19623,7 @@
         <v>387</v>
       </c>
       <c r="D221" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E221" s="8" t="s">
         <v>365</v>
@@ -19626,7 +19648,7 @@
         <v>389</v>
       </c>
       <c r="D222" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E222" s="8" t="s">
         <v>365</v>
@@ -19655,7 +19677,7 @@
         <v>393</v>
       </c>
       <c r="D223" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E223" s="8" t="s">
         <v>365</v>
@@ -19684,7 +19706,7 @@
         <v>394</v>
       </c>
       <c r="D224" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E224" s="8" t="s">
         <v>365</v>
@@ -19713,7 +19735,7 @@
         <v>394</v>
       </c>
       <c r="D225" s="29" t="s">
-        <v>311</v>
+        <v>839</v>
       </c>
       <c r="E225" s="8" t="s">
         <v>365</v>
@@ -41554,11 +41576,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:J38 I40:J40 I42:J42 I44:J44 I46:J46 I50:J50 I52:J52 I56:J56 I64:J64 I71:J71 I73:J73 I84:J84">
-    <cfRule type="cellIs" dxfId="90" priority="12" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="11" stopIfTrue="1" operator="greaterThan">
+      <formula>123256</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="12" stopIfTrue="1" operator="greaterThan">
       <formula>100000</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="11" stopIfTrue="1" operator="greaterThan">
-      <formula>123256</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39:J39">
@@ -41587,11 +41609,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48:J48">
-    <cfRule type="cellIs" dxfId="83" priority="23" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="22" stopIfTrue="1" operator="greaterThan">
+      <formula>123256</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="23" stopIfTrue="1" operator="greaterThan">
       <formula>100000</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="22" stopIfTrue="1" operator="greaterThan">
-      <formula>123256</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53:J53">
@@ -41600,19 +41622,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54:J54">
-    <cfRule type="cellIs" dxfId="80" priority="26" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="27" stopIfTrue="1" operator="greaterThan">
+      <formula>100000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="26" stopIfTrue="1" operator="greaterThan">
       <formula>123256</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="27" stopIfTrue="1" operator="greaterThan">
-      <formula>100000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I58:J58">
-    <cfRule type="cellIs" dxfId="78" priority="28" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="29" stopIfTrue="1" operator="greaterThan">
+      <formula>100000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="28" stopIfTrue="1" operator="greaterThan">
       <formula>123256</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="29" stopIfTrue="1" operator="greaterThan">
-      <formula>100000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I60:J60">
@@ -41691,11 +41713,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I78:J78">
-    <cfRule type="cellIs" dxfId="59" priority="58" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="59" stopIfTrue="1" operator="greaterThan">
+      <formula>100000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="58" stopIfTrue="1" operator="greaterThan">
       <formula>123256</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="59" stopIfTrue="1" operator="greaterThan">
-      <formula>100000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I79:J79">
@@ -41704,11 +41726,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I80:J80">
-    <cfRule type="cellIs" dxfId="56" priority="63" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="62" stopIfTrue="1" operator="greaterThan">
+      <formula>123256</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="63" stopIfTrue="1" operator="greaterThan">
       <formula>100000</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="62" stopIfTrue="1" operator="greaterThan">
-      <formula>123256</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81:J81">
@@ -41717,11 +41739,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I82:J82">
-    <cfRule type="cellIs" dxfId="53" priority="67" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="66" stopIfTrue="1" operator="greaterThan">
+      <formula>123256</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="67" stopIfTrue="1" operator="greaterThan">
       <formula>100000</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="66" stopIfTrue="1" operator="greaterThan">
-      <formula>123256</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I83:J83">
@@ -41730,11 +41752,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I87:J87">
-    <cfRule type="cellIs" dxfId="50" priority="72" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="73" stopIfTrue="1" operator="greaterThan">
+      <formula>100000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="72" stopIfTrue="1" operator="greaterThan">
       <formula>123256</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="73" stopIfTrue="1" operator="greaterThan">
-      <formula>100000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I88:J88">
@@ -41756,11 +41778,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I91:J91">
-    <cfRule type="cellIs" dxfId="44" priority="80" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="81" stopIfTrue="1" operator="greaterThan">
+      <formula>100000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="80" stopIfTrue="1" operator="greaterThan">
       <formula>123256</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="81" stopIfTrue="1" operator="greaterThan">
-      <formula>100000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I92:J92">
@@ -41907,11 +41929,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB40 AB43 AB46 AB49 AB52 AB55 AB58 AB61 AB64 AB67 AB69 AB72 AB75 AB77 AB80 AB83 AB88 AB91 AB94 AB97 AB100 AB103 AB106 AB109">
-    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="greaterThan">
+      <formula>100000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="greaterThan">
       <formula>123256</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="greaterThan">
-      <formula>100000</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="10">

</xml_diff>